<commit_message>
update gait results after fixing downsampling issues
</commit_message>
<xml_diff>
--- a/test/gait/data/manual_gait_turn_results.xlsx
+++ b/test/gait/data/manual_gait_turn_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/test/gait/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4A9037-DA69-A94A-8AD8-BD48CF120085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EAA7A8-50C8-2444-8452-CE5D327652EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19820" yWindow="500" windowWidth="48980" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:AI59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -570,7 +570,7 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="J2">
-        <v>6.702580323874259E-2</v>
+        <v>6.8329323533755995E-2</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -752,27 +752,27 @@
       </c>
       <c r="AC2">
         <f>2*SQRT(2 * L2 * J2 - J2 * J2)</f>
-        <v>0.71854453555605746</v>
+        <v>0.7252524511740398</v>
       </c>
       <c r="AD2">
         <f>AC3-AC2</f>
-        <v>8.9634722842377168E-2</v>
+        <v>-5.0120489936965051E-2</v>
       </c>
       <c r="AE2">
         <f>AC3+AC2</f>
-        <v>1.526723793954492</v>
+        <v>1.4003844124111144</v>
       </c>
       <c r="AF2">
         <f>AE3-AE2</f>
-        <v>3.8069521273984996E-2</v>
+        <v>5.9942299005819155E-2</v>
       </c>
       <c r="AG2">
         <f>AE2/O2</f>
-        <v>1.2938337236902475</v>
+        <v>1.1867664511958598</v>
       </c>
       <c r="AH2">
         <f>AG3-AG2</f>
-        <v>0.12870565379018606</v>
+        <v>0.1408032864558979</v>
       </c>
       <c r="AI2">
         <f>60/M2</f>
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="J3">
-        <v>8.5617626667248772E-2</v>
+        <v>5.8923510305967597E-2</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -882,27 +882,27 @@
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC58" si="16">2*SQRT(2 * L3 * J3 - J3 * J3)</f>
-        <v>0.80817925839843463</v>
+        <v>0.67513196123707475</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD57" si="17">AC4-AC3</f>
-        <v>-5.1565201568392172E-2</v>
+        <v>0.1100627889427841</v>
       </c>
       <c r="AE3">
         <f t="shared" ref="AE3:AE57" si="18">AC4+AC3</f>
-        <v>1.564793315228477</v>
+        <v>1.4603267114169336</v>
       </c>
       <c r="AF3">
         <f t="shared" ref="AF3:AF56" si="19">AE4-AE3</f>
-        <v>-5.3907454654512854E-2</v>
+        <v>9.9780603134010271E-2</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG57" si="20">AE3/O3</f>
-        <v>1.4225393774804336</v>
+        <v>1.3275697376517577</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH56" si="21">AG4-AG3</f>
-        <v>2.8246419289663649E-3</v>
+        <v>0.14422961569818926</v>
       </c>
       <c r="AI3">
         <f t="shared" ref="AI3:AI58" si="22">60/M3</f>
@@ -938,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <v>7.4610028123653166E-2</v>
+        <v>8.0605120634267099E-2</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1012,27 +1012,27 @@
       </c>
       <c r="AC4">
         <f t="shared" si="16"/>
-        <v>0.75661405683004246</v>
+        <v>0.78519475017985885</v>
       </c>
       <c r="AD4">
         <f t="shared" si="17"/>
-        <v>-2.3422530861206825E-3</v>
+        <v>-1.0282185808773714E-2</v>
       </c>
       <c r="AE4">
         <f t="shared" si="18"/>
-        <v>1.5108858605739641</v>
+        <v>1.5601073145509439</v>
       </c>
       <c r="AF4">
         <f t="shared" si="19"/>
-        <v>2.9246024784836955E-3</v>
+        <v>-1.9463409410700017E-2</v>
       </c>
       <c r="AG4">
         <f t="shared" si="20"/>
-        <v>1.4253640194093999</v>
+        <v>1.4717993533499469</v>
       </c>
       <c r="AH4">
         <f t="shared" si="21"/>
-        <v>-2.3687664731207647E-2</v>
+        <v>-4.5277218960832366E-2</v>
       </c>
       <c r="AI4">
         <f t="shared" si="22"/>
@@ -1068,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="J5">
-        <v>7.4130260976094528E-2</v>
+        <v>7.8418197677667903E-2</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1142,27 +1142,27 @@
       </c>
       <c r="AC5">
         <f t="shared" si="16"/>
-        <v>0.75427180374392178</v>
+        <v>0.77491256437108513</v>
       </c>
       <c r="AD5">
         <f t="shared" si="17"/>
-        <v>5.2668555646041559E-3</v>
+        <v>-9.1812236019265248E-3</v>
       </c>
       <c r="AE5">
         <f t="shared" si="18"/>
-        <v>1.5138104630524478</v>
+        <v>1.5406439051402439</v>
       </c>
       <c r="AF5">
         <f t="shared" si="19"/>
-        <v>8.2125917795110581E-3</v>
+        <v>-1.9870153940506619E-2</v>
       </c>
       <c r="AG5">
         <f t="shared" si="20"/>
-        <v>1.4016763546781923</v>
+        <v>1.4265221343891146</v>
       </c>
       <c r="AH5">
         <f t="shared" si="21"/>
-        <v>-1.8019032103684385E-2</v>
+        <v>-4.400054238935347E-2</v>
       </c>
       <c r="AI5">
         <f t="shared" si="22"/>
@@ -1198,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="J6">
-        <v>7.5211519691028864E-2</v>
+        <v>7.6494114356818202E-2</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1272,27 +1272,27 @@
       </c>
       <c r="AC6">
         <f t="shared" si="16"/>
-        <v>0.75953865930852593</v>
+        <v>0.76573134076915861</v>
       </c>
       <c r="AD6">
         <f t="shared" si="17"/>
-        <v>2.9457362149069022E-3</v>
+        <v>-1.0688930338580094E-2</v>
       </c>
       <c r="AE6">
         <f t="shared" si="18"/>
-        <v>1.5220230548319589</v>
+        <v>1.5207737511997372</v>
       </c>
       <c r="AF6">
         <f t="shared" si="19"/>
-        <v>7.1825106523036419E-2</v>
+        <v>7.3138362247022748E-2</v>
       </c>
       <c r="AG6">
         <f t="shared" si="20"/>
-        <v>1.3836573225745079</v>
+        <v>1.3825215919997611</v>
       </c>
       <c r="AH6">
         <f t="shared" si="21"/>
-        <v>6.5295551384578543E-2</v>
+        <v>6.6489420224566054E-2</v>
       </c>
       <c r="AI6">
         <f t="shared" si="22"/>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="J7">
-        <v>7.5820103062305466E-2</v>
+        <v>7.4287913747577303E-2</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1402,27 +1402,27 @@
       </c>
       <c r="AC7">
         <f t="shared" si="16"/>
-        <v>0.76248439552343283</v>
+        <v>0.75504241043057851</v>
       </c>
       <c r="AD7">
         <f t="shared" si="17"/>
-        <v>6.8879370308129628E-2</v>
+        <v>8.3827292585602842E-2</v>
       </c>
       <c r="AE7">
         <f t="shared" si="18"/>
-        <v>1.5938481613549953</v>
+        <v>1.59391211344676</v>
       </c>
       <c r="AF7">
         <f t="shared" si="19"/>
-        <v>-2.132840858418894E-2</v>
+        <v>-7.6672713040979446E-3</v>
       </c>
       <c r="AG7">
         <f t="shared" si="20"/>
-        <v>1.4489528739590865</v>
+        <v>1.4490110122243272</v>
       </c>
       <c r="AH7">
         <f t="shared" si="21"/>
-        <v>-9.3332397432529079E-2</v>
+        <v>-8.1558562101342602E-2</v>
       </c>
       <c r="AI7">
         <f t="shared" si="22"/>
@@ -1458,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="J8">
-        <v>9.0849597087168915E-2</v>
+        <v>9.2581785235335098E-2</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1532,27 +1532,27 @@
       </c>
       <c r="AC8">
         <f t="shared" si="16"/>
-        <v>0.83136376583156246</v>
+        <v>0.83886970301618136</v>
       </c>
       <c r="AD8">
         <f t="shared" si="17"/>
-        <v>-9.020777889231868E-2</v>
+        <v>-9.1494563889700675E-2</v>
       </c>
       <c r="AE8">
         <f t="shared" si="18"/>
-        <v>1.5725197527708064</v>
+        <v>1.586244842142662</v>
       </c>
       <c r="AF8">
         <f t="shared" si="19"/>
-        <v>-0.23187537045149664</v>
+        <v>-0.2353442515311519</v>
       </c>
       <c r="AG8">
         <f t="shared" si="20"/>
-        <v>1.3556204765265574</v>
+        <v>1.3674524501229846</v>
       </c>
       <c r="AH8">
         <f t="shared" si="21"/>
-        <v>-0.21948116947629481</v>
+        <v>-0.22262144113017923</v>
       </c>
       <c r="AI8">
         <f t="shared" si="22"/>
@@ -1588,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="J9">
-        <v>7.1475727015433504E-2</v>
+        <v>7.2727676957938497E-2</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1662,27 +1662,27 @@
       </c>
       <c r="AC9">
         <f t="shared" si="16"/>
-        <v>0.74115598693924378</v>
+        <v>0.74737513912648068</v>
       </c>
       <c r="AD9">
         <f t="shared" si="17"/>
-        <v>-0.14166759155917785</v>
+        <v>-0.14384968764145123</v>
       </c>
       <c r="AE9">
         <f t="shared" si="18"/>
-        <v>1.3406443823193097</v>
+        <v>1.3509005906115101</v>
       </c>
       <c r="AF9">
         <f t="shared" si="19"/>
-        <v>-0.12993984824769766</v>
+        <v>-0.1551506827473248</v>
       </c>
       <c r="AG9">
         <f t="shared" si="20"/>
-        <v>1.1361393070502626</v>
+        <v>1.1448310089928053</v>
       </c>
       <c r="AH9">
         <f t="shared" si="21"/>
-        <v>-0.11011851546415063</v>
+        <v>-0.13148362944688552</v>
       </c>
       <c r="AI9">
         <f t="shared" si="22"/>
@@ -1718,7 +1718,7 @@
         <v>3</v>
       </c>
       <c r="J10">
-        <v>4.6154570675997188E-2</v>
+        <v>4.6793651373134598E-2</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -1792,27 +1792,27 @@
       </c>
       <c r="AC10">
         <f t="shared" si="16"/>
-        <v>0.59948839538006593</v>
+        <v>0.60352545148502945</v>
       </c>
       <c r="AD10">
         <f t="shared" si="17"/>
-        <v>1.1727743311480299E-2</v>
+        <v>-1.1300995105873568E-2</v>
       </c>
       <c r="AE10">
         <f t="shared" si="18"/>
-        <v>1.210704534071612</v>
+        <v>1.1957499078641853</v>
       </c>
       <c r="AF10">
         <f t="shared" si="19"/>
-        <v>2.119317970464385E-2</v>
+        <v>2.2920343597504722E-2</v>
       </c>
       <c r="AG10">
         <f t="shared" si="20"/>
-        <v>1.0260207915861119</v>
+        <v>1.0133473795459198</v>
       </c>
       <c r="AH10">
         <f t="shared" si="21"/>
-        <v>5.459123804218291E-2</v>
+        <v>5.5661612964334806E-2</v>
       </c>
       <c r="AI10">
         <f t="shared" si="22"/>
@@ -1848,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="J11">
-        <v>4.8024194767312123E-2</v>
+        <v>4.5016529302404101E-2</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -1922,27 +1922,27 @@
       </c>
       <c r="AC11">
         <f t="shared" si="16"/>
-        <v>0.61121613869154623</v>
+        <v>0.59222445637915588</v>
       </c>
       <c r="AD11">
         <f t="shared" si="17"/>
-        <v>9.465436393163551E-3</v>
+        <v>3.422133870337829E-2</v>
       </c>
       <c r="AE11">
         <f t="shared" si="18"/>
-        <v>1.2318977137762559</v>
+        <v>1.2186702514616901</v>
       </c>
       <c r="AF11">
         <f t="shared" si="19"/>
-        <v>0.2332014818672592</v>
+        <v>0.27096654812079612</v>
       </c>
       <c r="AG11">
         <f t="shared" si="20"/>
-        <v>1.0806120296282948</v>
+        <v>1.0690089925102546</v>
       </c>
       <c r="AH11">
         <f t="shared" si="21"/>
-        <v>0.27596129967125616</v>
+        <v>0.31028434043649167</v>
       </c>
       <c r="AI11">
         <f t="shared" si="22"/>
@@ -1978,7 +1978,7 @@
         <v>3</v>
       </c>
       <c r="J12">
-        <v>4.9562339369841633E-2</v>
+        <v>5.0511858380784598E-2</v>
       </c>
       <c r="K12">
         <v>2</v>
@@ -2052,27 +2052,27 @@
       </c>
       <c r="AC12">
         <f t="shared" si="16"/>
-        <v>0.62068157508470978</v>
+        <v>0.62644579508253417</v>
       </c>
       <c r="AD12">
         <f t="shared" si="17"/>
-        <v>0.22373604547409542</v>
+        <v>0.23674520941741783</v>
       </c>
       <c r="AE12">
         <f t="shared" si="18"/>
-        <v>1.4650991956435151</v>
+        <v>1.4896367995824862</v>
       </c>
       <c r="AF12">
         <f t="shared" si="19"/>
-        <v>0.15763010859553228</v>
+        <v>0.15410859989547787</v>
       </c>
       <c r="AG12">
         <f t="shared" si="20"/>
-        <v>1.356573329299551</v>
+        <v>1.3792933329467463</v>
       </c>
       <c r="AH12">
         <f t="shared" si="21"/>
-        <v>0.11863512909958285</v>
+        <v>0.11502066657867549</v>
       </c>
       <c r="AI12">
         <f t="shared" si="22"/>
@@ -2108,7 +2108,7 @@
         <v>3</v>
       </c>
       <c r="J13">
-        <v>9.3874277085438745E-2</v>
+        <v>9.8325235608086495E-2</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -2182,27 +2182,27 @@
       </c>
       <c r="AC13">
         <f t="shared" si="16"/>
-        <v>0.8444176205588052</v>
+        <v>0.86319100449995201</v>
       </c>
       <c r="AD13">
         <f t="shared" si="17"/>
-        <v>-6.6105936878563143E-2</v>
+        <v>-8.2636609521939852E-2</v>
       </c>
       <c r="AE13">
         <f t="shared" si="18"/>
-        <v>1.6227293042390474</v>
+        <v>1.6437453994779641</v>
       </c>
       <c r="AF13">
         <f t="shared" si="19"/>
-        <v>-4.9801172123755233E-2</v>
+        <v>-4.92647917908422E-2</v>
       </c>
       <c r="AG13">
         <f t="shared" si="20"/>
-        <v>1.4752084583991338</v>
+        <v>1.4943139995254218</v>
       </c>
       <c r="AH13">
         <f t="shared" si="21"/>
-        <v>-1.8793521255344947E-2</v>
+        <v>-1.7943066481790559E-2</v>
       </c>
       <c r="AI13">
         <f t="shared" si="22"/>
@@ -2238,7 +2238,7 @@
         <v>3</v>
       </c>
       <c r="J14">
-        <v>7.9137392694051484E-2</v>
+        <v>7.9613945830256799E-2</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -2312,27 +2312,27 @@
       </c>
       <c r="AC14">
         <f t="shared" si="16"/>
-        <v>0.77831168368024206</v>
+        <v>0.78055439497801216</v>
       </c>
       <c r="AD14">
         <f t="shared" si="17"/>
-        <v>1.6304764754808132E-2</v>
+        <v>3.3371817731097653E-2</v>
       </c>
       <c r="AE14">
         <f t="shared" si="18"/>
-        <v>1.5729281321152921</v>
+        <v>1.5944806076871219</v>
       </c>
       <c r="AF14">
         <f t="shared" si="19"/>
-        <v>4.1903276592232697E-2</v>
+        <v>4.669841516299611E-2</v>
       </c>
       <c r="AG14">
         <f t="shared" si="20"/>
-        <v>1.4564149371437889</v>
+        <v>1.4763709330436312</v>
       </c>
       <c r="AH14">
         <f t="shared" si="21"/>
-        <v>6.7010920127460905E-2</v>
+        <v>7.1911163984781812E-2</v>
       </c>
       <c r="AI14">
         <f t="shared" si="22"/>
@@ -2368,7 +2368,7 @@
         <v>3</v>
       </c>
       <c r="J15">
-        <v>8.2639016498780027E-2</v>
+        <v>8.6897943891136004E-2</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -2442,27 +2442,27 @@
       </c>
       <c r="AC15">
         <f t="shared" si="16"/>
-        <v>0.79461644843505019</v>
+        <v>0.81392621270910981</v>
       </c>
       <c r="AD15">
         <f t="shared" si="17"/>
-        <v>2.5598511837424343E-2</v>
+        <v>1.3326597431898457E-2</v>
       </c>
       <c r="AE15">
         <f t="shared" si="18"/>
-        <v>1.6148314087075248</v>
+        <v>1.641179022850118</v>
       </c>
       <c r="AF15">
         <f t="shared" si="19"/>
-        <v>3.3225956609925111E-2</v>
+        <v>5.5321235146357672E-2</v>
       </c>
       <c r="AG15">
         <f t="shared" si="20"/>
-        <v>1.5234258572712498</v>
+        <v>1.548282097028413</v>
       </c>
       <c r="AH15">
         <f t="shared" si="21"/>
-        <v>2.5531846893518395E-3</v>
+        <v>2.2551475190545789E-2</v>
       </c>
       <c r="AI15">
         <f t="shared" si="22"/>
@@ -2498,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="J16">
-        <v>8.8311449947580417E-2</v>
+        <v>8.9908876475642899E-2</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -2572,27 +2572,27 @@
       </c>
       <c r="AC16">
         <f t="shared" si="16"/>
-        <v>0.82021496027247454</v>
+        <v>0.82725281014100827</v>
       </c>
       <c r="AD16">
         <f t="shared" si="17"/>
-        <v>7.6274447725008798E-3</v>
+        <v>4.1994637714459215E-2</v>
       </c>
       <c r="AE16">
         <f t="shared" si="18"/>
-        <v>1.64805736531745</v>
+        <v>1.6965002579964756</v>
       </c>
       <c r="AF16">
         <f t="shared" si="19"/>
-        <v>3.4790973943636949E-3</v>
+        <v>3.0207202745536677E-2</v>
       </c>
       <c r="AG16">
         <f t="shared" si="20"/>
-        <v>1.5259790419606016</v>
+        <v>1.5708335722189588</v>
       </c>
       <c r="AH16">
         <f t="shared" si="21"/>
-        <v>-2.4582257677134844E-2</v>
+        <v>-1.0995169989478359E-3</v>
       </c>
       <c r="AI16">
         <f t="shared" si="22"/>
@@ -2628,7 +2628,7 @@
         <v>3</v>
       </c>
       <c r="J17">
-        <v>9.0043448690120792E-2</v>
+        <v>9.9786828894874502E-2</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -2702,27 +2702,27 @@
       </c>
       <c r="AC17">
         <f t="shared" si="16"/>
-        <v>0.82784240504497542</v>
+        <v>0.86924744785546748</v>
       </c>
       <c r="AD17">
         <f t="shared" si="17"/>
-        <v>-4.1483473781371849E-3</v>
+        <v>-1.1787434968922539E-2</v>
       </c>
       <c r="AE17">
         <f t="shared" si="18"/>
-        <v>1.6515364627118136</v>
+        <v>1.7267074607420123</v>
       </c>
       <c r="AF17">
         <f t="shared" si="19"/>
-        <v>-0.15467373811169938</v>
+        <v>-0.19158487304248562</v>
       </c>
       <c r="AG17">
         <f t="shared" si="20"/>
-        <v>1.5013967842834668</v>
+        <v>1.569734055220011</v>
       </c>
       <c r="AH17">
         <f t="shared" si="21"/>
-        <v>-0.14061248919245384</v>
+        <v>-0.17416806640225957</v>
       </c>
       <c r="AI17">
         <f t="shared" si="22"/>
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="J18">
-        <v>8.9099065997899005E-2</v>
+        <v>9.6953758373991797E-2</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2832,27 +2832,27 @@
       </c>
       <c r="AC18">
         <f t="shared" si="16"/>
-        <v>0.82369405766683823</v>
+        <v>0.85746001288654494</v>
       </c>
       <c r="AD18">
         <f t="shared" si="17"/>
-        <v>-0.15052539073356208</v>
+        <v>-0.17979743807356319</v>
       </c>
       <c r="AE18">
         <f t="shared" si="18"/>
-        <v>1.4968627246001143</v>
+        <v>1.5351225876995267</v>
       </c>
       <c r="AF18">
         <f t="shared" si="19"/>
-        <v>-0.14194884278869013</v>
+        <v>-0.17220109500584169</v>
       </c>
       <c r="AG18">
         <f t="shared" si="20"/>
-        <v>1.360784295091013</v>
+        <v>1.3955659888177514</v>
       </c>
       <c r="AH18">
         <f t="shared" si="21"/>
-        <v>-0.17226334613362315</v>
+        <v>-0.20002081978820296</v>
       </c>
       <c r="AI18">
         <f t="shared" si="22"/>
@@ -2888,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="J19">
-        <v>5.85706197474836E-2</v>
+        <v>5.9380086297809803E-2</v>
       </c>
       <c r="K19">
         <v>2</v>
@@ -2962,27 +2962,27 @@
       </c>
       <c r="AC19">
         <f t="shared" si="16"/>
-        <v>0.67316866693327615</v>
+        <v>0.67766257481298176</v>
       </c>
       <c r="AD19">
         <f t="shared" si="17"/>
-        <v>8.5765479448718374E-3</v>
+        <v>7.5963430677215005E-3</v>
       </c>
       <c r="AE19">
         <f t="shared" si="18"/>
-        <v>1.3549138818114241</v>
+        <v>1.362921492693685</v>
       </c>
       <c r="AF19" s="3">
         <f t="shared" si="19"/>
-        <v>-0.67316866693327615</v>
+        <v>-0.67766257481298176</v>
       </c>
       <c r="AG19">
         <f t="shared" si="20"/>
-        <v>1.1885209489573898</v>
+        <v>1.1955451690295484</v>
       </c>
       <c r="AH19" s="3">
         <f t="shared" si="21"/>
-        <v>-1.0277319831842417</v>
+        <v>-1.0339274997180619</v>
       </c>
       <c r="AI19">
         <f t="shared" si="22"/>
@@ -3018,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>6.0120754530099102E-2</v>
+        <v>6.0762242175829102E-2</v>
       </c>
       <c r="K20">
         <v>2</v>
@@ -3092,27 +3092,27 @@
       </c>
       <c r="AC20">
         <f t="shared" si="16"/>
-        <v>0.68174521487814799</v>
+        <v>0.68525891788070326</v>
       </c>
       <c r="AD20" s="3">
         <f t="shared" si="17"/>
-        <v>-0.68174521487814799</v>
+        <v>-0.68525891788070326</v>
       </c>
       <c r="AE20" s="3">
         <f t="shared" si="18"/>
-        <v>0.68174521487814799</v>
+        <v>0.68525891788070326</v>
       </c>
       <c r="AF20" s="3">
         <f t="shared" si="19"/>
-        <v>4.2804233313189721E-2</v>
+        <v>3.2500810056777074E-2</v>
       </c>
       <c r="AG20" s="3">
         <f t="shared" si="20"/>
-        <v>0.16078896577314811</v>
+        <v>0.16161766931148661</v>
       </c>
       <c r="AH20" s="3">
         <f t="shared" si="21"/>
-        <v>1.0095338045563618E-2</v>
+        <v>7.6652853907493157E-3</v>
       </c>
       <c r="AI20">
         <f t="shared" si="22"/>
@@ -3223,23 +3223,23 @@
       </c>
       <c r="AD21" s="3">
         <f t="shared" si="17"/>
-        <v>0.72454944819133771</v>
+        <v>0.71775972793748033</v>
       </c>
       <c r="AE21" s="3">
         <f t="shared" si="18"/>
-        <v>0.72454944819133771</v>
+        <v>0.71775972793748033</v>
       </c>
       <c r="AF21" s="3">
         <f t="shared" si="19"/>
-        <v>0.74613638857327103</v>
+        <v>0.7769222731266423</v>
       </c>
       <c r="AG21" s="3">
         <f t="shared" si="20"/>
-        <v>0.17088430381871172</v>
+        <v>0.16928295470223592</v>
       </c>
       <c r="AH21" s="3">
         <f t="shared" si="21"/>
-        <v>1.1191909915888398</v>
+        <v>1.141841607634714</v>
       </c>
       <c r="AI21" s="3">
         <f t="shared" si="22"/>
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
       <c r="J22">
-        <v>6.8192057628568351E-2</v>
+        <v>6.6874205178910295E-2</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -3349,27 +3349,27 @@
       </c>
       <c r="AC22">
         <f t="shared" si="16"/>
-        <v>0.72454944819133771</v>
+        <v>0.71775972793748033</v>
       </c>
       <c r="AD22">
         <f t="shared" si="17"/>
-        <v>2.1586940381933428E-2</v>
+        <v>5.9162545189161864E-2</v>
       </c>
       <c r="AE22">
         <f t="shared" si="18"/>
-        <v>1.4706858367646087</v>
+        <v>1.4946820010641226</v>
       </c>
       <c r="AF22">
         <f t="shared" si="19"/>
-        <v>0.11390995747711896</v>
+        <v>0.15311846107161164</v>
       </c>
       <c r="AG22">
         <f t="shared" si="20"/>
-        <v>1.2900752954075516</v>
+        <v>1.3111245623369499</v>
       </c>
       <c r="AH22">
         <f t="shared" si="21"/>
-        <v>0.20482639727332352</v>
+        <v>0.24340417552695026</v>
       </c>
       <c r="AI22">
         <f t="shared" si="22"/>
@@ -3405,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="J23">
-        <v>7.2477339593995493E-2</v>
+        <v>7.8842968867911298E-2</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3479,27 +3479,27 @@
       </c>
       <c r="AC23">
         <f t="shared" si="16"/>
-        <v>0.74613638857327114</v>
+        <v>0.77692227312664219</v>
       </c>
       <c r="AD23">
         <f t="shared" si="17"/>
-        <v>9.2323017095185533E-2</v>
+        <v>9.3955915882449892E-2</v>
       </c>
       <c r="AE23">
         <f t="shared" si="18"/>
-        <v>1.5845957942417277</v>
+        <v>1.6478004621357343</v>
       </c>
       <c r="AF23">
         <f t="shared" si="19"/>
-        <v>0.10961816225136656</v>
+        <v>0.11649196784140603</v>
       </c>
       <c r="AG23">
         <f t="shared" si="20"/>
-        <v>1.4949016926808751</v>
+        <v>1.5545287378639001</v>
       </c>
       <c r="AH23">
         <f t="shared" si="21"/>
-        <v>0.10341336061449669</v>
+        <v>0.10989808286925107</v>
       </c>
       <c r="AI23">
         <f t="shared" si="22"/>
@@ -3535,7 +3535,7 @@
         <v>3</v>
       </c>
       <c r="J24">
-        <v>9.2486610199005531E-2</v>
+        <v>0.10018252919447</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -3609,27 +3609,27 @@
       </c>
       <c r="AC24">
         <f t="shared" si="16"/>
-        <v>0.83845940566845667</v>
+        <v>0.87087818900909209</v>
       </c>
       <c r="AD24">
         <f t="shared" si="17"/>
-        <v>1.7295145156180913E-2</v>
+        <v>2.2536051958956027E-2</v>
       </c>
       <c r="AE24">
         <f t="shared" si="18"/>
-        <v>1.6942139564930943</v>
+        <v>1.7642924299771403</v>
       </c>
       <c r="AF24">
         <f t="shared" si="19"/>
-        <v>1.0873218848708843E-2</v>
+        <v>1.1936377879873561E-2</v>
       </c>
       <c r="AG24">
         <f t="shared" si="20"/>
-        <v>1.5983150532953718</v>
+        <v>1.6644268207331512</v>
       </c>
       <c r="AH24">
         <f t="shared" si="21"/>
-        <v>1.0257753630857458E-2</v>
+        <v>1.1260733848937221E-2</v>
       </c>
       <c r="AI24">
         <f t="shared" si="22"/>
@@ -3665,7 +3665,7 @@
         <v>3</v>
       </c>
       <c r="J25">
-        <v>9.654779147588316E-2</v>
+        <v>0.105745348348266</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -3739,27 +3739,27 @@
       </c>
       <c r="AC25">
         <f t="shared" si="16"/>
-        <v>0.85575455082463758</v>
+        <v>0.89341424096804811</v>
       </c>
       <c r="AD25">
         <f t="shared" si="17"/>
-        <v>-6.4219263074721811E-3</v>
+        <v>-1.0599674079082244E-2</v>
       </c>
       <c r="AE25">
         <f t="shared" si="18"/>
-        <v>1.7050871753418031</v>
+        <v>1.7762288078570139</v>
       </c>
       <c r="AF25">
         <f t="shared" si="19"/>
-        <v>1.0747755706172146E-2</v>
+        <v>3.0545982111860326E-3</v>
       </c>
       <c r="AG25">
         <f t="shared" si="20"/>
-        <v>1.6085728069262293</v>
+        <v>1.6756875545820884</v>
       </c>
       <c r="AH25">
         <f t="shared" si="21"/>
-        <v>1.0139392175634088E-2</v>
+        <v>2.8816964256472843E-3</v>
       </c>
       <c r="AI25">
         <f t="shared" si="22"/>
@@ -3795,7 +3795,7 @@
         <v>3</v>
       </c>
       <c r="J26">
-        <v>9.5027999529219934E-2</v>
+        <v>0.103106895737932</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -3869,27 +3869,27 @@
       </c>
       <c r="AC26">
         <f t="shared" si="16"/>
-        <v>0.8493326245171654</v>
+        <v>0.88281456688896587</v>
       </c>
       <c r="AD26">
         <f t="shared" si="17"/>
-        <v>1.7169682013644549E-2</v>
+        <v>1.3654272290268166E-2</v>
       </c>
       <c r="AE26">
         <f t="shared" si="18"/>
-        <v>1.7158349310479752</v>
+        <v>1.7792834060681999</v>
       </c>
       <c r="AF26">
         <f t="shared" si="19"/>
-        <v>-8.3668584262637236E-2</v>
+        <v>-0.11170878762957193</v>
       </c>
       <c r="AG26">
         <f t="shared" si="20"/>
-        <v>1.6187121991018634</v>
+        <v>1.6785692510077357</v>
       </c>
       <c r="AH26">
         <f t="shared" si="21"/>
-        <v>-0.16142081804352593</v>
+        <v>-0.18966334168753218</v>
       </c>
       <c r="AI26">
         <f t="shared" si="22"/>
@@ -3925,7 +3925,7 @@
         <v>3</v>
       </c>
       <c r="J27">
-        <v>9.9122786317296166E-2</v>
+        <v>0.106513004311694</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -3999,27 +3999,27 @@
       </c>
       <c r="AC27">
         <f t="shared" si="16"/>
-        <v>0.86650230653080995</v>
+        <v>0.89646883917923403</v>
       </c>
       <c r="AD27">
         <f t="shared" si="17"/>
-        <v>-0.10083826627628201</v>
+        <v>-0.12536305991983998</v>
       </c>
       <c r="AE27">
         <f t="shared" si="18"/>
-        <v>1.632166346785338</v>
+        <v>1.667574618438628</v>
       </c>
       <c r="AF27">
         <f t="shared" si="19"/>
-        <v>-0.16575053003344831</v>
+        <v>-0.18874863807499853</v>
       </c>
       <c r="AG27">
         <f t="shared" si="20"/>
-        <v>1.4572913810583374</v>
+        <v>1.4889059093202035</v>
       </c>
       <c r="AH27">
         <f t="shared" si="21"/>
-        <v>-0.21456611262453262</v>
+        <v>-0.23566355307983944</v>
       </c>
       <c r="AI27">
         <f t="shared" si="22"/>
@@ -4055,7 +4055,7 @@
         <v>3</v>
       </c>
       <c r="J28">
-        <v>7.6480109811034605E-2</v>
+        <v>7.7617147908064898E-2</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -4129,27 +4129,27 @@
       </c>
       <c r="AC28">
         <f t="shared" si="16"/>
-        <v>0.76566404025452794</v>
+        <v>0.77110577925939405</v>
       </c>
       <c r="AD28">
         <f t="shared" si="17"/>
-        <v>-6.4912263757166078E-2</v>
+        <v>-6.3385578155158551E-2</v>
       </c>
       <c r="AE28">
         <f t="shared" si="18"/>
-        <v>1.4664158167518897</v>
+        <v>1.4788259803636294</v>
       </c>
       <c r="AF28">
         <f t="shared" si="19"/>
-        <v>-0.21835964715799983</v>
+        <v>-0.22252786442490446</v>
       </c>
       <c r="AG28">
         <f t="shared" si="20"/>
-        <v>1.2427252684338048</v>
+        <v>1.2532423562403641</v>
       </c>
       <c r="AH28">
         <f t="shared" si="21"/>
-        <v>-0.20267846043889648</v>
+        <v>-0.20632725962475984</v>
       </c>
       <c r="AI28">
         <f t="shared" si="22"/>
@@ -4185,7 +4185,7 @@
         <v>3</v>
       </c>
       <c r="J29">
-        <v>6.3635454718637005E-2</v>
+        <v>6.4951671193058003E-2</v>
       </c>
       <c r="K29">
         <v>2</v>
@@ -4259,27 +4259,27 @@
       </c>
       <c r="AC29">
         <f t="shared" si="16"/>
-        <v>0.70075177649736187</v>
+        <v>0.7077202011042355</v>
       </c>
       <c r="AD29">
         <f t="shared" si="17"/>
-        <v>-0.15344738340083386</v>
+        <v>-0.15914228626974591</v>
       </c>
       <c r="AE29">
         <f t="shared" si="18"/>
-        <v>1.2480561695938899</v>
+        <v>1.256298115938725</v>
       </c>
       <c r="AF29">
         <f t="shared" si="19"/>
-        <v>-0.25779633849279482</v>
+        <v>-0.27137310365630873</v>
       </c>
       <c r="AG29">
         <f t="shared" si="20"/>
-        <v>1.0400468079949083</v>
+        <v>1.0469150966156042</v>
       </c>
       <c r="AH29">
         <f t="shared" si="21"/>
-        <v>-0.24145017001015423</v>
+        <v>-0.25262073187172018</v>
       </c>
       <c r="AI29">
         <f t="shared" si="22"/>
@@ -4315,7 +4315,7 @@
         <v>3</v>
       </c>
       <c r="J30">
-        <v>3.831470352357965E-2</v>
+        <v>3.8496806645389202E-2</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -4389,27 +4389,27 @@
       </c>
       <c r="AC30">
         <f t="shared" si="16"/>
-        <v>0.54730439309652801</v>
+        <v>0.54857791483448959</v>
       </c>
       <c r="AD30">
         <f t="shared" si="17"/>
-        <v>-0.1043489550919609</v>
+        <v>-0.11223081738656288</v>
       </c>
       <c r="AE30">
         <f t="shared" si="18"/>
-        <v>0.99025983110109506</v>
+        <v>0.98492501228241625</v>
       </c>
       <c r="AF30">
         <f t="shared" si="19"/>
-        <v>4.9319885126134055E-2</v>
+        <v>5.061870440773153E-2</v>
       </c>
       <c r="AG30">
         <f t="shared" si="20"/>
-        <v>0.79859663798475411</v>
+        <v>0.79429436474388404</v>
       </c>
       <c r="AH30">
         <f t="shared" si="21"/>
-        <v>6.7719792204603557E-2</v>
+        <v>6.8658732497905772E-2</v>
       </c>
       <c r="AI30">
         <f t="shared" si="22"/>
@@ -4445,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="J31">
-        <v>2.492659326899456E-2</v>
+        <v>2.41792109622463E-2</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -4519,27 +4519,27 @@
       </c>
       <c r="AC31">
         <f t="shared" si="16"/>
-        <v>0.4429554380045671</v>
+        <v>0.43634709744792671</v>
       </c>
       <c r="AD31">
         <f t="shared" si="17"/>
-        <v>0.15366884021809485</v>
+        <v>0.16284952179429441</v>
       </c>
       <c r="AE31">
         <f t="shared" si="18"/>
-        <v>1.0395797162272291</v>
+        <v>1.0355437166901478</v>
       </c>
       <c r="AF31">
         <f t="shared" si="19"/>
-        <v>0.31368014382450649</v>
+        <v>0.34622331041115406</v>
       </c>
       <c r="AG31">
         <f t="shared" si="20"/>
-        <v>0.86631643018935767</v>
+        <v>0.86295309724178981</v>
       </c>
       <c r="AH31">
         <f t="shared" si="21"/>
-        <v>0.32075362248760342</v>
+        <v>0.34912324232075576</v>
       </c>
       <c r="AI31">
         <f t="shared" si="22"/>
@@ -4575,7 +4575,7 @@
         <v>3</v>
       </c>
       <c r="J32">
-        <v>4.5704029850330161E-2</v>
+        <v>4.6108564243487901E-2</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -4649,27 +4649,27 @@
       </c>
       <c r="AC32">
         <f t="shared" si="16"/>
-        <v>0.59662427822266195</v>
+        <v>0.59919661924222112</v>
       </c>
       <c r="AD32">
         <f t="shared" si="17"/>
-        <v>0.16001130360641169</v>
+        <v>0.1833737886168596</v>
       </c>
       <c r="AE32">
         <f t="shared" si="18"/>
-        <v>1.3532598600517356</v>
+        <v>1.3817670271013018</v>
       </c>
       <c r="AF32">
         <f t="shared" si="19"/>
-        <v>0.16348547646675238</v>
+        <v>0.15500361874056567</v>
       </c>
       <c r="AG32">
         <f t="shared" si="20"/>
-        <v>1.1870700526769611</v>
+        <v>1.2120763395625456</v>
       </c>
       <c r="AH32">
         <f t="shared" si="21"/>
-        <v>0.14340831269013377</v>
+        <v>0.13596808661453141</v>
       </c>
       <c r="AI32">
         <f t="shared" si="22"/>
@@ -4705,7 +4705,7 @@
         <v>3</v>
       </c>
       <c r="J33">
-        <v>7.4614445178519409E-2</v>
+        <v>8.0043710565689402E-2</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -4779,27 +4779,27 @@
       </c>
       <c r="AC33">
         <f t="shared" si="16"/>
-        <v>0.75663558182907364</v>
+        <v>0.78257040785908072</v>
       </c>
       <c r="AD33">
         <f t="shared" si="17"/>
-        <v>3.4741728603407962E-3</v>
+        <v>-2.8370169876293927E-2</v>
       </c>
       <c r="AE33">
         <f t="shared" si="18"/>
-        <v>1.516745336518488</v>
+        <v>1.5367706458418675</v>
       </c>
       <c r="AF33">
         <f t="shared" si="19"/>
-        <v>0.11510023997198404</v>
+        <v>0.1329260056003998</v>
       </c>
       <c r="AG33">
         <f t="shared" si="20"/>
-        <v>1.3304783653670949</v>
+        <v>1.348044426177077</v>
       </c>
       <c r="AH33">
         <f t="shared" si="21"/>
-        <v>0.15301761326060692</v>
+        <v>0.16986162058862053</v>
       </c>
       <c r="AI33">
         <f t="shared" si="22"/>
@@ -4835,7 +4835,7 @@
         <v>3</v>
       </c>
       <c r="J34">
-        <v>7.5329291418677502E-2</v>
+        <v>7.4115629398027294E-2</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -4909,27 +4909,27 @@
       </c>
       <c r="AC34">
         <f t="shared" si="16"/>
-        <v>0.76010975468941444</v>
+        <v>0.75420023798278679</v>
       </c>
       <c r="AD34">
         <f t="shared" si="17"/>
-        <v>0.11162606711164313</v>
+        <v>0.16129617547669362</v>
       </c>
       <c r="AE34">
         <f t="shared" si="18"/>
-        <v>1.631845576490472</v>
+        <v>1.6696966514422673</v>
       </c>
       <c r="AF34">
         <f t="shared" si="19"/>
-        <v>2.1436427409115666E-2</v>
+        <v>5.3778654339927456E-2</v>
       </c>
       <c r="AG34">
         <f t="shared" si="20"/>
-        <v>1.4834959786277018</v>
+        <v>1.5179060467656975</v>
       </c>
       <c r="AH34">
         <f t="shared" si="21"/>
-        <v>4.7320691649694213E-2</v>
+        <v>7.7904421551149294E-2</v>
       </c>
       <c r="AI34">
         <f t="shared" si="22"/>
@@ -4965,7 +4965,7 @@
         <v>3</v>
       </c>
       <c r="J35">
-        <v>0.10039100213937099</v>
+        <v>0.111369187408875</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -5039,27 +5039,27 @@
       </c>
       <c r="AC35">
         <f t="shared" si="16"/>
-        <v>0.87173582180105758</v>
+        <v>0.91549641345948041</v>
       </c>
       <c r="AD35">
         <f t="shared" si="17"/>
-        <v>-9.018963970252758E-2</v>
+        <v>-0.10751752113676616</v>
       </c>
       <c r="AE35">
         <f t="shared" si="18"/>
-        <v>1.6532820038995877</v>
+        <v>1.7234753057821948</v>
       </c>
       <c r="AF35">
         <f t="shared" si="19"/>
-        <v>-1.1995710176043062E-2</v>
+        <v>-3.1551650875558668E-2</v>
       </c>
       <c r="AG35">
         <f t="shared" si="20"/>
-        <v>1.530816670277396</v>
+        <v>1.5958104683168468</v>
       </c>
       <c r="AH35">
         <f t="shared" si="21"/>
-        <v>1.7566625688212101E-2</v>
+        <v>3.4392310450792607E-4</v>
       </c>
       <c r="AI35">
         <f t="shared" si="22"/>
@@ -5095,7 +5095,7 @@
         <v>3</v>
       </c>
       <c r="J36">
-        <v>7.9825206918822778E-2</v>
+        <v>8.5573184743532094E-2</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -5169,27 +5169,27 @@
       </c>
       <c r="AC36">
         <f t="shared" si="16"/>
-        <v>0.78154618209853</v>
+        <v>0.80797889232271425</v>
       </c>
       <c r="AD36">
         <f t="shared" si="17"/>
-        <v>7.8193929526484518E-2</v>
+        <v>7.5965870261207491E-2</v>
       </c>
       <c r="AE36">
         <f t="shared" si="18"/>
-        <v>1.6412862937235446</v>
+        <v>1.6919236549066361</v>
       </c>
       <c r="AF36">
         <f t="shared" si="19"/>
-        <v>-1.4962178629907896E-2</v>
+        <v>-7.4707325396077273E-3</v>
       </c>
       <c r="AG36">
         <f t="shared" si="20"/>
-        <v>1.5483832959656081</v>
+        <v>1.5961543914213547</v>
       </c>
       <c r="AH36">
         <f t="shared" si="21"/>
-        <v>-4.2527633841870527E-2</v>
+        <v>-3.6475759600032243E-2</v>
       </c>
       <c r="AI36">
         <f t="shared" si="22"/>
@@ -5225,7 +5225,7 @@
         <v>3</v>
       </c>
       <c r="J37">
-        <v>9.7498061457340121E-2</v>
+        <v>0.103386352749795</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -5299,27 +5299,27 @@
       </c>
       <c r="AC37">
         <f t="shared" si="16"/>
-        <v>0.85974011162501451</v>
+        <v>0.88394476258392174</v>
       </c>
       <c r="AD37">
         <f t="shared" si="17"/>
-        <v>-9.3156108156392303E-2</v>
+        <v>-8.3436602800815107E-2</v>
       </c>
       <c r="AE37">
         <f t="shared" si="18"/>
-        <v>1.6263241150936367</v>
+        <v>1.6844529223670284</v>
       </c>
       <c r="AF37">
         <f t="shared" si="19"/>
-        <v>-0.10895206476950681</v>
+        <v>-0.13292986119253047</v>
       </c>
       <c r="AG37">
         <f t="shared" si="20"/>
-        <v>1.5058556621237376</v>
+        <v>1.5596786318213225</v>
       </c>
       <c r="AH37">
         <f t="shared" si="21"/>
-        <v>-0.1510591886200503</v>
+        <v>-0.17439018434409226</v>
       </c>
       <c r="AI37">
         <f t="shared" si="22"/>
@@ -5355,7 +5355,7 @@
         <v>2</v>
       </c>
       <c r="J38">
-        <v>7.6671669781502888E-2</v>
+        <v>8.3925544724584605E-2</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -5429,27 +5429,27 @@
       </c>
       <c r="AC38">
         <f t="shared" si="16"/>
-        <v>0.76658400346862221</v>
+        <v>0.80050815978310663</v>
       </c>
       <c r="AD38">
         <f t="shared" si="17"/>
-        <v>-1.5795956613114503E-2</v>
+        <v>-4.9493258391715367E-2</v>
       </c>
       <c r="AE38">
         <f t="shared" si="18"/>
-        <v>1.5173720503241299</v>
+        <v>1.5515230611744979</v>
       </c>
       <c r="AF38" s="3">
         <f t="shared" si="19"/>
-        <v>-0.76658400346862221</v>
+        <v>-0.80050815978310663</v>
       </c>
       <c r="AG38">
         <f t="shared" si="20"/>
-        <v>1.3547964735036873</v>
+        <v>1.3852884474772302</v>
       </c>
       <c r="AH38" s="3">
         <f t="shared" si="21"/>
-        <v>-1.1622867178997109</v>
+        <v>-1.1927205240435401</v>
       </c>
       <c r="AI38">
         <f t="shared" si="22"/>
@@ -5485,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="J39">
-        <v>7.3419887985270299E-2</v>
+        <v>7.3466029191676302E-2</v>
       </c>
       <c r="K39">
         <v>2</v>
@@ -5559,27 +5559,27 @@
       </c>
       <c r="AC39">
         <f t="shared" si="16"/>
-        <v>0.75078804685550771</v>
+        <v>0.75101490139139127</v>
       </c>
       <c r="AD39" s="3">
         <f t="shared" si="17"/>
-        <v>-0.75078804685550771</v>
+        <v>-0.75101490139139127</v>
       </c>
       <c r="AE39" s="3">
         <f t="shared" si="18"/>
-        <v>0.75078804685550771</v>
+        <v>0.75101490139139127</v>
       </c>
       <c r="AF39" s="3">
         <f t="shared" si="19"/>
-        <v>1.1658186468960885E-2</v>
+        <v>2.3919467291382945E-2</v>
       </c>
       <c r="AG39" s="3">
         <f t="shared" si="20"/>
-        <v>0.19250975560397635</v>
+        <v>0.19256792343369009</v>
       </c>
       <c r="AH39" s="3">
         <f t="shared" si="21"/>
-        <v>1.0045168134014681E-3</v>
+        <v>4.1159264857957567E-3</v>
       </c>
       <c r="AI39">
         <f t="shared" si="22"/>
@@ -5690,23 +5690,23 @@
       </c>
       <c r="AD40" s="3">
         <f t="shared" si="17"/>
-        <v>0.76244623332446859</v>
+        <v>0.77493436868277421</v>
       </c>
       <c r="AE40" s="3">
         <f t="shared" si="18"/>
-        <v>0.76244623332446859</v>
+        <v>0.77493436868277421</v>
       </c>
       <c r="AF40" s="3">
         <f t="shared" si="19"/>
-        <v>0.79811603876317183</v>
+        <v>0.82935884840194729</v>
       </c>
       <c r="AG40" s="3">
         <f t="shared" si="20"/>
-        <v>0.19351427241737781</v>
+        <v>0.19668384991948584</v>
       </c>
       <c r="AH40" s="3">
         <f t="shared" si="21"/>
-        <v>1.1754000013437105</v>
+        <v>1.2105909019092174</v>
       </c>
       <c r="AI40" s="3">
         <f t="shared" si="22"/>
@@ -5742,7 +5742,7 @@
         <v>3</v>
       </c>
       <c r="J41">
-        <v>7.581220118756056E-2</v>
+        <v>7.8422799270832899E-2</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -5816,27 +5816,27 @@
       </c>
       <c r="AC41">
         <f t="shared" si="16"/>
-        <v>0.76244623332446859</v>
+        <v>0.77493436868277421</v>
       </c>
       <c r="AD41">
         <f t="shared" si="17"/>
-        <v>3.5669805438703239E-2</v>
+        <v>5.4424479719172969E-2</v>
       </c>
       <c r="AE41">
         <f t="shared" si="18"/>
-        <v>1.5605622720876404</v>
+        <v>1.6042932170847215</v>
       </c>
       <c r="AF41">
         <f t="shared" si="19"/>
-        <v>5.5667765171389494E-2</v>
+        <v>5.6259348056255876E-2</v>
       </c>
       <c r="AG41">
         <f t="shared" si="20"/>
-        <v>1.3689142737610882</v>
+        <v>1.4072747518287032</v>
       </c>
       <c r="AH41">
         <f t="shared" si="21"/>
-        <v>0.12759501999727263</v>
+        <v>0.13027391959812751</v>
       </c>
       <c r="AI41">
         <f t="shared" si="22"/>
@@ -5872,7 +5872,7 @@
         <v>3</v>
       </c>
       <c r="J42">
-        <v>8.3401830687900122E-2</v>
+        <v>9.0390102071534195E-2</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -5946,27 +5946,27 @@
       </c>
       <c r="AC42">
         <f t="shared" si="16"/>
-        <v>0.79811603876317183</v>
+        <v>0.82935884840194718</v>
       </c>
       <c r="AD42">
         <f t="shared" si="17"/>
-        <v>1.9997959732686144E-2</v>
+        <v>1.8348683370830177E-3</v>
       </c>
       <c r="AE42">
         <f t="shared" si="18"/>
-        <v>1.6162300372590299</v>
+        <v>1.6605525651409774</v>
       </c>
       <c r="AF42">
         <f t="shared" si="19"/>
-        <v>4.4911332239052637E-2</v>
+        <v>3.4495358160637979E-2</v>
       </c>
       <c r="AG42">
         <f t="shared" si="20"/>
-        <v>1.4965092937583608</v>
+        <v>1.5375486714268307</v>
       </c>
       <c r="AH42">
         <f t="shared" si="21"/>
-        <v>7.0605205768132118E-2</v>
+        <v>6.1553143008655331E-2</v>
       </c>
       <c r="AI42">
         <f t="shared" si="22"/>
@@ -6002,7 +6002,7 @@
         <v>3</v>
       </c>
       <c r="J43">
-        <v>8.783776692717421E-2</v>
+        <v>9.08105724372721E-2</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -6076,27 +6076,27 @@
       </c>
       <c r="AC43">
         <f t="shared" si="16"/>
-        <v>0.81811399849585797</v>
+        <v>0.8311937167390302</v>
       </c>
       <c r="AD43">
         <f t="shared" si="17"/>
-        <v>2.4913372506366604E-2</v>
+        <v>3.2660489823555072E-2</v>
       </c>
       <c r="AE43">
         <f t="shared" si="18"/>
-        <v>1.6611413694980826</v>
+        <v>1.6950479233016154</v>
       </c>
       <c r="AF43">
         <f t="shared" si="19"/>
-        <v>3.6434836149124683E-2</v>
+        <v>5.4199202926513479E-2</v>
       </c>
       <c r="AG43">
         <f t="shared" si="20"/>
-        <v>1.567114499526493</v>
+        <v>1.599101814435486</v>
       </c>
       <c r="AH43">
         <f t="shared" si="21"/>
-        <v>6.5170313595821705E-2</v>
+        <v>8.2866576168483919E-2</v>
       </c>
       <c r="AI43">
         <f t="shared" si="22"/>
@@ -6132,7 +6132,7 @@
         <v>3</v>
       </c>
       <c r="J44">
-        <v>9.3549418267192236E-2</v>
+        <v>9.8484671335302601E-2</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -6206,27 +6206,27 @@
       </c>
       <c r="AC44">
         <f t="shared" si="16"/>
-        <v>0.84302737100222458</v>
+        <v>0.86385420656258527</v>
       </c>
       <c r="AD44">
         <f t="shared" si="17"/>
-        <v>1.1521463642758079E-2</v>
+        <v>2.1538713102958185E-2</v>
       </c>
       <c r="AE44">
         <f t="shared" si="18"/>
-        <v>1.6975762056472072</v>
+        <v>1.7492471262281288</v>
       </c>
       <c r="AF44">
         <f t="shared" si="19"/>
-        <v>-4.9117201664160115E-2</v>
+        <v>-4.6800447814761892E-2</v>
       </c>
       <c r="AG44">
         <f t="shared" si="20"/>
-        <v>1.6322848131223147</v>
+        <v>1.68196839060397</v>
       </c>
       <c r="AH44">
         <f t="shared" si="21"/>
-        <v>-7.7134809364723056E-2</v>
+        <v>-7.588661851588796E-2</v>
       </c>
       <c r="AI44">
         <f t="shared" si="22"/>
@@ -6262,7 +6262,7 @@
         <v>3</v>
       </c>
       <c r="J45">
-        <v>9.6261381618516759E-2</v>
+        <v>0.10374508097948</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -6336,27 +6336,27 @@
       </c>
       <c r="AC45">
         <f t="shared" si="16"/>
-        <v>0.85454883464498266</v>
+        <v>0.88539291966554345</v>
       </c>
       <c r="AD45">
         <f t="shared" si="17"/>
-        <v>-6.0638665306918083E-2</v>
+        <v>-6.8339160917719965E-2</v>
       </c>
       <c r="AE45">
         <f t="shared" si="18"/>
-        <v>1.6484590039830471</v>
+        <v>1.7024466784133669</v>
       </c>
       <c r="AF45">
         <f t="shared" si="19"/>
-        <v>-2.9807934776141076E-2</v>
+        <v>-3.5567137226821144E-2</v>
       </c>
       <c r="AG45">
         <f t="shared" si="20"/>
-        <v>1.5551500037575916</v>
+        <v>1.606081772088082</v>
       </c>
       <c r="AH45">
         <f t="shared" si="21"/>
-        <v>-8.3649031751313441E-2</v>
+        <v>-9.0736734645767703E-2</v>
       </c>
       <c r="AI45">
         <f t="shared" si="22"/>
@@ -6392,7 +6392,7 @@
         <v>3</v>
       </c>
       <c r="J46">
-        <v>8.2485550636493418E-2</v>
+        <v>8.7599279913900305E-2</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -6466,27 +6466,27 @@
       </c>
       <c r="AC46">
         <f t="shared" si="16"/>
-        <v>0.79391016933806458</v>
+        <v>0.81705375874782349</v>
       </c>
       <c r="AD46">
         <f t="shared" si="17"/>
-        <v>3.0830730530776895E-2</v>
+        <v>3.2772023690898822E-2</v>
       </c>
       <c r="AE46">
         <f t="shared" si="18"/>
-        <v>1.618651069206906</v>
+        <v>1.6668795411865458</v>
       </c>
       <c r="AF46">
         <f t="shared" si="19"/>
-        <v>2.5316922764788474E-2</v>
+        <v>2.4612580515969817E-2</v>
       </c>
       <c r="AG46">
         <f t="shared" si="20"/>
-        <v>1.4715009720062782</v>
+        <v>1.5153450374423143</v>
       </c>
       <c r="AH46">
         <f t="shared" si="21"/>
-        <v>-5.428718582378278E-2</v>
+        <v>-5.7162173905662916E-2</v>
       </c>
       <c r="AI46">
         <f t="shared" si="22"/>
@@ -6522,7 +6522,7 @@
         <v>3</v>
       </c>
       <c r="J47">
-        <v>8.933684231974047E-2</v>
+        <v>9.5144212292867805E-2</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -6596,27 +6596,27 @@
       </c>
       <c r="AC47">
         <f t="shared" si="16"/>
-        <v>0.82474089986884147</v>
+        <v>0.84982578243872231</v>
       </c>
       <c r="AD47">
         <f t="shared" si="17"/>
-        <v>-5.513807765988421E-3</v>
+        <v>-8.1594431749290042E-3</v>
       </c>
       <c r="AE47">
         <f t="shared" si="18"/>
-        <v>1.6439679919716945</v>
+        <v>1.6914921217025156</v>
       </c>
       <c r="AF47">
         <f t="shared" si="19"/>
-        <v>-0.14451978539071231</v>
+        <v>-0.12994830966268434</v>
       </c>
       <c r="AG47">
         <f t="shared" si="20"/>
-        <v>1.4172137861824954</v>
+        <v>1.4581828635366514</v>
       </c>
       <c r="AH47">
         <f t="shared" si="21"/>
-        <v>-0.14649496704606979</v>
+        <v>-0.13484064994357392</v>
       </c>
       <c r="AI47">
         <f t="shared" si="22"/>
@@ -6652,7 +6652,7 @@
         <v>3</v>
       </c>
       <c r="J48">
-        <v>8.8088543014470264E-2</v>
+        <v>9.3232018206152706E-2</v>
       </c>
       <c r="K48">
         <v>1</v>
@@ -6726,27 +6726,27 @@
       </c>
       <c r="AC48">
         <f t="shared" si="16"/>
-        <v>0.81922709210285305</v>
+        <v>0.84166633926379331</v>
       </c>
       <c r="AD48">
         <f t="shared" si="17"/>
-        <v>-0.139005977624724</v>
+        <v>-0.12178886648775522</v>
       </c>
       <c r="AE48">
         <f t="shared" si="18"/>
-        <v>1.4994482065809822</v>
+        <v>1.5615438120398313</v>
       </c>
       <c r="AF48">
         <f t="shared" si="19"/>
-        <v>-0.27079781105249179</v>
+        <v>-0.27433902396029342</v>
       </c>
       <c r="AG48">
         <f t="shared" si="20"/>
-        <v>1.2707188191364256</v>
+        <v>1.3233422135930775</v>
       </c>
       <c r="AH48">
         <f t="shared" si="21"/>
-        <v>-0.32560313026835608</v>
+        <v>-0.33318468430112524</v>
       </c>
       <c r="AI48">
         <f t="shared" si="22"/>
@@ -6782,7 +6782,7 @@
         <v>3</v>
       </c>
       <c r="J49">
-        <v>5.9843664879398191E-2</v>
+        <v>6.7283717693314704E-2</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -6856,27 +6856,27 @@
       </c>
       <c r="AC49">
         <f t="shared" si="16"/>
-        <v>0.68022111447812905</v>
+        <v>0.71987747277603809</v>
       </c>
       <c r="AD49">
         <f t="shared" si="17"/>
-        <v>-0.13179183342776757</v>
+        <v>-0.15255015747253831</v>
       </c>
       <c r="AE49">
         <f t="shared" si="18"/>
-        <v>1.2286503955284904</v>
+        <v>1.2872047880795379</v>
       </c>
       <c r="AF49">
         <f t="shared" si="19"/>
-        <v>-0.11244087782502965</v>
+        <v>-0.15861523504534536</v>
       </c>
       <c r="AG49">
         <f t="shared" si="20"/>
-        <v>0.94511568886806951</v>
+        <v>0.99015752929195222</v>
       </c>
       <c r="AH49">
         <f t="shared" si="21"/>
-        <v>-5.9235119262148306E-2</v>
+        <v>-9.445153482037083E-2</v>
       </c>
       <c r="AI49">
         <f t="shared" si="22"/>
@@ -6912,7 +6912,7 @@
         <v>3</v>
       </c>
       <c r="J50">
-        <v>3.8475529636263071E-2</v>
+        <v>4.1230962955964102E-2</v>
       </c>
       <c r="K50">
         <v>2</v>
@@ -6986,27 +6986,27 @@
       </c>
       <c r="AC50">
         <f t="shared" si="16"/>
-        <v>0.54842928105036148</v>
+        <v>0.56732731530349978</v>
       </c>
       <c r="AD50">
         <f t="shared" si="17"/>
-        <v>1.9350955602737807E-2</v>
+        <v>-6.0650775728069428E-3</v>
       </c>
       <c r="AE50">
         <f t="shared" si="18"/>
-        <v>1.1162095177034608</v>
+        <v>1.1285895530341925</v>
       </c>
       <c r="AF50">
         <f t="shared" si="19"/>
-        <v>0.22394049418934547</v>
+        <v>0.21934260633701985</v>
       </c>
       <c r="AG50">
         <f t="shared" si="20"/>
-        <v>0.88588056960592121</v>
+        <v>0.89570599447158139</v>
       </c>
       <c r="AH50">
         <f t="shared" si="21"/>
-        <v>0.28968961626496148</v>
+        <v>0.28669063655579807</v>
       </c>
       <c r="AI50">
         <f t="shared" si="22"/>
@@ -7042,7 +7042,7 @@
         <v>3</v>
       </c>
       <c r="J51">
-        <v>4.1298245883435912E-2</v>
+        <v>4.0335600953375197E-2</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -7116,27 +7116,27 @@
       </c>
       <c r="AC51">
         <f t="shared" si="16"/>
-        <v>0.56778023665309929</v>
+        <v>0.56126223773069284</v>
       </c>
       <c r="AD51">
         <f t="shared" si="17"/>
-        <v>0.20458953858660756</v>
+        <v>0.22540768390982668</v>
       </c>
       <c r="AE51">
         <f t="shared" si="18"/>
-        <v>1.3401500118928062</v>
+        <v>1.3479321593712124</v>
       </c>
       <c r="AF51">
         <f t="shared" si="19"/>
-        <v>0.16917768554139379</v>
+        <v>0.19826804144052623</v>
       </c>
       <c r="AG51">
         <f t="shared" si="20"/>
-        <v>1.1755701858708827</v>
+        <v>1.1823966310273795</v>
       </c>
       <c r="AH51">
         <f t="shared" si="21"/>
-        <v>0.10352108314115127</v>
+        <v>0.12794252220290758</v>
       </c>
       <c r="AI51">
         <f t="shared" si="22"/>
@@ -7172,7 +7172,7 @@
         <v>3</v>
       </c>
       <c r="J52">
-        <v>7.7882611719276629E-2</v>
+        <v>8.0921672240940101E-2</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -7246,27 +7246,27 @@
       </c>
       <c r="AC52">
         <f t="shared" si="16"/>
-        <v>0.77236977523970685</v>
+        <v>0.78666992164051952</v>
       </c>
       <c r="AD52">
         <f t="shared" si="17"/>
-        <v>-3.541185304521377E-2</v>
+        <v>-2.713964246930034E-2</v>
       </c>
       <c r="AE52">
         <f t="shared" si="18"/>
-        <v>1.5093276974342</v>
+        <v>1.5462002008117386</v>
       </c>
       <c r="AF52">
         <f t="shared" si="19"/>
-        <v>5.2520106685013612E-2</v>
+        <v>3.2008147846189328E-2</v>
       </c>
       <c r="AG52">
         <f t="shared" si="20"/>
-        <v>1.279091269012034</v>
+        <v>1.310339153230287</v>
       </c>
       <c r="AH52">
         <f t="shared" si="21"/>
-        <v>0.11541569895154957</v>
+        <v>9.8775443785719785E-2</v>
       </c>
       <c r="AI52">
         <f t="shared" si="22"/>
@@ -7302,7 +7302,7 @@
         <v>3</v>
       </c>
       <c r="J53">
-        <v>7.0637495235039302E-2</v>
+        <v>7.5209792303716202E-2</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -7376,27 +7376,27 @@
       </c>
       <c r="AC53">
         <f t="shared" si="16"/>
-        <v>0.73695792219449308</v>
+        <v>0.75953027917121918</v>
       </c>
       <c r="AD53">
         <f t="shared" si="17"/>
-        <v>8.7931959730227383E-2</v>
+        <v>5.9147790315489668E-2</v>
       </c>
       <c r="AE53">
         <f t="shared" si="18"/>
-        <v>1.5618478041192136</v>
+        <v>1.5782083486579279</v>
       </c>
       <c r="AF53">
         <f t="shared" si="19"/>
-        <v>0.11518091471182168</v>
+        <v>0.13175647692565673</v>
       </c>
       <c r="AG53">
         <f t="shared" si="20"/>
-        <v>1.3945069679635835</v>
+        <v>1.4091145970160068</v>
       </c>
       <c r="AH53">
         <f t="shared" si="21"/>
-        <v>0.1300645946100849</v>
+        <v>0.14539888078725172</v>
       </c>
       <c r="AI53">
         <f t="shared" si="22"/>
@@ -7432,7 +7432,7 @@
         <v>3</v>
       </c>
       <c r="J54">
-        <v>8.9370711236646333E-2</v>
+        <v>8.7964798879205205E-2</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -7506,27 +7506,27 @@
       </c>
       <c r="AC54">
         <f t="shared" si="16"/>
-        <v>0.82488988192472046</v>
+        <v>0.81867806948670885</v>
       </c>
       <c r="AD54">
         <f t="shared" si="17"/>
-        <v>2.7248954981594409E-2</v>
+        <v>7.260868661016695E-2</v>
       </c>
       <c r="AE54">
         <f t="shared" si="18"/>
-        <v>1.6770287188310353</v>
+        <v>1.7099648255835846</v>
       </c>
       <c r="AF54">
         <f t="shared" si="19"/>
-        <v>-5.6840457580373815E-2</v>
+        <v>-4.8646642424683195E-2</v>
       </c>
       <c r="AG54">
         <f t="shared" si="20"/>
-        <v>1.5245715625736684</v>
+        <v>1.5545134778032585</v>
       </c>
       <c r="AH54">
         <f t="shared" si="21"/>
-        <v>-2.4397246600833755E-2</v>
+        <v>-1.6255900804275747E-2</v>
       </c>
       <c r="AI54">
         <f t="shared" si="22"/>
@@ -7562,7 +7562,7 @@
         <v>3</v>
       </c>
       <c r="J55">
-        <v>9.5690384941412868E-2</v>
+        <v>0.105212623742023</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -7636,27 +7636,27 @@
       </c>
       <c r="AC55">
         <f t="shared" si="16"/>
-        <v>0.85213883690631487</v>
+        <v>0.8912867560968758</v>
       </c>
       <c r="AD55">
         <f t="shared" si="17"/>
-        <v>-8.4089412561968224E-2</v>
+        <v>-0.12125532903485015</v>
       </c>
       <c r="AE55">
         <f t="shared" si="18"/>
-        <v>1.6201882612506615</v>
+        <v>1.6613181831589015</v>
       </c>
       <c r="AF55">
         <f t="shared" si="19"/>
-        <v>-2.4339980285523088E-2</v>
+        <v>-4.3329936082568299E-2</v>
       </c>
       <c r="AG55">
         <f t="shared" si="20"/>
-        <v>1.5001743159728347</v>
+        <v>1.5382575769989828</v>
       </c>
       <c r="AH55">
         <f t="shared" si="21"/>
-        <v>-2.2537018782891716E-2</v>
+        <v>-4.0120311187563207E-2</v>
       </c>
       <c r="AI55">
         <f t="shared" si="22"/>
@@ -7692,7 +7692,7 @@
         <v>3</v>
       </c>
       <c r="J56">
-        <v>7.6977365712003254E-2</v>
+        <v>7.73919149788697E-2</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -7766,27 +7766,27 @@
       </c>
       <c r="AC56">
         <f t="shared" si="16"/>
-        <v>0.76804942434434664</v>
+        <v>0.77003142706202565</v>
       </c>
       <c r="AD56">
         <f t="shared" si="17"/>
-        <v>5.9749432276445025E-2</v>
+        <v>7.7925392952281847E-2</v>
       </c>
       <c r="AE56">
         <f t="shared" si="18"/>
-        <v>1.5958482809651384</v>
+        <v>1.6179882470763332</v>
       </c>
       <c r="AF56">
         <f t="shared" si="19"/>
-        <v>-2.7691345414028845E-2</v>
+        <v>-5.1935690789890021E-2</v>
       </c>
       <c r="AG56">
         <f t="shared" si="20"/>
-        <v>1.477637297189943</v>
+        <v>1.4981372658114196</v>
       </c>
       <c r="AH56">
         <f t="shared" si="21"/>
-        <v>-7.7497176162166781E-2</v>
+        <v>-9.987605484138129E-2</v>
       </c>
       <c r="AI56">
         <f t="shared" si="22"/>
@@ -7822,7 +7822,7 @@
         <v>2</v>
       </c>
       <c r="J57">
-        <v>9.0033505007865208E-2</v>
+        <v>9.4704226555427498E-2</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -7890,20 +7890,20 @@
       </c>
       <c r="AC57">
         <f t="shared" si="16"/>
-        <v>0.82779885662079167</v>
+        <v>0.8479568200143075</v>
       </c>
       <c r="AD57">
         <f t="shared" si="17"/>
-        <v>-8.744077769047387E-2</v>
+        <v>-0.12986108374217176</v>
       </c>
       <c r="AE57">
         <f t="shared" si="18"/>
-        <v>1.5681569355511096</v>
+        <v>1.5660525562864431</v>
       </c>
       <c r="AF57" s="3"/>
       <c r="AG57">
         <f t="shared" si="20"/>
-        <v>1.4001401210277762</v>
+        <v>1.3982612109700383</v>
       </c>
       <c r="AH57" s="3"/>
       <c r="AI57">
@@ -7938,7 +7938,7 @@
         <v>1</v>
       </c>
       <c r="J58">
-        <v>7.131598287471623E-2</v>
+        <v>6.69390872194007E-2</v>
       </c>
       <c r="K58">
         <v>2</v>
@@ -7988,7 +7988,7 @@
       <c r="AB58" s="3"/>
       <c r="AC58">
         <f t="shared" si="16"/>
-        <v>0.7403580789303178</v>
+        <v>0.71809573627213574</v>
       </c>
       <c r="AD58" s="3"/>
       <c r="AE58" s="3"/>

</xml_diff>